<commit_message>
added field end time in report
</commit_message>
<xml_diff>
--- a/work_plan_report.xlsx
+++ b/work_plan_report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>&lt; Program Name &gt;</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Día</t>
   </si>
   <si>
-    <t>Horario</t>
-  </si>
-  <si>
     <t>Distribución</t>
   </si>
   <si>
@@ -64,6 +61,12 @@
   </si>
   <si>
     <t>Profesor/Área/Sesión</t>
+  </si>
+  <si>
+    <t>Comienzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final </t>
   </si>
 </sst>
 </file>
@@ -586,14 +589,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -637,7 +640,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="9" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title 2" xfId="41" customBuiltin="1"/>
+    <cellStyle name="Title 2" xfId="41"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -650,13 +653,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>2071914</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>158115</xdr:rowOff>
@@ -991,70 +994,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
       <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:6" ht="15.75">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:6" ht="15.75">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>